<commit_message>
Added cross tabulation functions
</commit_message>
<xml_diff>
--- a/Exchange_Rate.xlsx
+++ b/Exchange_Rate.xlsx
@@ -458,10 +458,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="3">
-        <v>44534</v>
+        <v>44536</v>
       </c>
       <c r="E2">
-        <v>1638576002</v>
+        <v>1638748801</v>
       </c>
       <c r="F2">
         <v>3.67</v>
@@ -478,13 +478,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="3">
-        <v>44534</v>
+        <v>44536</v>
       </c>
       <c r="E3">
-        <v>1638576002</v>
+        <v>1638748801</v>
       </c>
       <c r="F3">
-        <v>96.17</v>
+        <v>96.25</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -498,13 +498,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="3">
-        <v>44534</v>
+        <v>44536</v>
       </c>
       <c r="E4">
-        <v>1638576002</v>
+        <v>1638748801</v>
       </c>
       <c r="F4">
-        <v>107.02</v>
+        <v>107.26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -518,13 +518,13 @@
         <v>11</v>
       </c>
       <c r="D5" s="3">
-        <v>44534</v>
+        <v>44536</v>
       </c>
       <c r="E5">
-        <v>1638576002</v>
+        <v>1638748801</v>
       </c>
       <c r="F5">
-        <v>489.42</v>
+        <v>489.44</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -538,10 +538,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="3">
-        <v>44534</v>
+        <v>44536</v>
       </c>
       <c r="E6">
-        <v>1638576002</v>
+        <v>1638748801</v>
       </c>
       <c r="F6">
         <v>1.79</v>

</xml_diff>

<commit_message>
Added pandas on spark with PySpark module
</commit_message>
<xml_diff>
--- a/Exchange_Rate.xlsx
+++ b/Exchange_Rate.xlsx
@@ -458,10 +458,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="3">
-        <v>44537</v>
+        <v>44574</v>
       </c>
       <c r="E2">
-        <v>1638835201</v>
+        <v>1642032001</v>
       </c>
       <c r="F2">
         <v>3.67</v>
@@ -478,13 +478,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="3">
-        <v>44537</v>
+        <v>44574</v>
       </c>
       <c r="E3">
-        <v>1638835201</v>
+        <v>1642032001</v>
       </c>
       <c r="F3">
-        <v>96.25</v>
+        <v>105.37</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -498,13 +498,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="3">
-        <v>44537</v>
+        <v>44574</v>
       </c>
       <c r="E4">
-        <v>1638835201</v>
+        <v>1642032001</v>
       </c>
       <c r="F4">
-        <v>107.1</v>
+        <v>107.13</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -518,13 +518,13 @@
         <v>11</v>
       </c>
       <c r="D5" s="3">
-        <v>44537</v>
+        <v>44574</v>
       </c>
       <c r="E5">
-        <v>1638835201</v>
+        <v>1642032001</v>
       </c>
       <c r="F5">
-        <v>490.9</v>
+        <v>481.78</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -538,10 +538,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="3">
-        <v>44537</v>
+        <v>44574</v>
       </c>
       <c r="E6">
-        <v>1638835201</v>
+        <v>1642032001</v>
       </c>
       <c r="F6">
         <v>1.79</v>

</xml_diff>